<commit_message>
Update Konzeptueller Entwurf und Aufwandsschätzung
</commit_message>
<xml_diff>
--- a/Dokumente/Konzeptueller Entwurf/Aufwandsschätzung.xlsx
+++ b/Dokumente/Konzeptueller Entwurf/Aufwandsschätzung.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Anwender\Documents\GitHub\258321_DKE_PR\Dokumente\Konzeptueller Entwurf\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{458F7225-0424-4E85-9C33-524EA8EBCA19}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{756218BB-5646-4317-A505-B2A0C6F50F65}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7545" xr2:uid="{D4203D62-B900-4327-9FC4-747C9894F5FC}"/>
   </bookViews>
@@ -446,7 +446,7 @@
   <dimension ref="A1:B16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I13" sqref="I13"/>
+      <selection activeCell="D8" sqref="D8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -476,7 +476,7 @@
         <v>2</v>
       </c>
       <c r="B4">
-        <v>75</v>
+        <v>50</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
@@ -497,7 +497,7 @@
         <v>4</v>
       </c>
       <c r="B7">
-        <v>80</v>
+        <v>120</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.25">
@@ -505,7 +505,7 @@
         <v>5</v>
       </c>
       <c r="B8">
-        <v>80</v>
+        <v>100</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.25">
@@ -513,7 +513,7 @@
         <v>6</v>
       </c>
       <c r="B9">
-        <v>45</v>
+        <v>30</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.25">
@@ -521,7 +521,7 @@
         <v>7</v>
       </c>
       <c r="B10">
-        <v>30</v>
+        <v>50</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.25">
@@ -545,7 +545,7 @@
         <v>9</v>
       </c>
       <c r="B13">
-        <v>50</v>
+        <v>30</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.25">
@@ -553,7 +553,7 @@
         <v>10</v>
       </c>
       <c r="B14">
-        <v>50</v>
+        <v>30</v>
       </c>
     </row>
     <row r="15" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">

</xml_diff>

<commit_message>
Update Code + Präsentation
</commit_message>
<xml_diff>
--- a/Dokumente/Konzeptueller Entwurf/Aufwandsschätzung.xlsx
+++ b/Dokumente/Konzeptueller Entwurf/Aufwandsschätzung.xlsx
@@ -1,31 +1,40 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="19126"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20730"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Anwender\Documents\GitHub\258321_DKE_PR\Dokumente\Konzeptueller Entwurf\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{0C5D4415-05AA-47E4-A610-0CEB9C65B421}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{117018D8-E4E1-4999-B416-3552EF85923F}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7545" xr2:uid="{D4203D62-B900-4327-9FC4-747C9894F5FC}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7545" activeTab="1" xr2:uid="{D4203D62-B900-4327-9FC4-747C9894F5FC}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
+    <sheet name="Vergleich" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="179017"/>
+  <externalReferences>
+    <externalReference r:id="rId3"/>
+  </externalReferences>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="23">
   <si>
     <t xml:space="preserve">Aufwandsschätzung </t>
   </si>
@@ -85,6 +94,15 @@
   </si>
   <si>
     <t>Teuchtmann</t>
+  </si>
+  <si>
+    <t>Dusanic</t>
+  </si>
+  <si>
+    <t>Tomic</t>
+  </si>
+  <si>
+    <t>tatsächlich</t>
   </si>
 </sst>
 </file>
@@ -159,6 +177,536 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/externalLinks/externalLink1.xml><?xml version="1.0" encoding="utf-8"?>
+<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" mc:Ignorable="x14">
+  <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
+    <sheetNames>
+      <sheetName val="Zeiterfassung_Gesamt"/>
+      <sheetName val="Aistleithner"/>
+      <sheetName val="Dusanic"/>
+      <sheetName val="Teuchtmann"/>
+      <sheetName val="Tomic"/>
+    </sheetNames>
+    <sheetDataSet>
+      <sheetData sheetId="0" refreshError="1"/>
+      <sheetData sheetId="1">
+        <row r="8">
+          <cell r="G8">
+            <v>3</v>
+          </cell>
+        </row>
+        <row r="10">
+          <cell r="G10">
+            <v>2</v>
+          </cell>
+        </row>
+        <row r="11">
+          <cell r="G11">
+            <v>6</v>
+          </cell>
+        </row>
+        <row r="12">
+          <cell r="G12">
+            <v>1.5</v>
+          </cell>
+        </row>
+        <row r="14">
+          <cell r="G14">
+            <v>2</v>
+          </cell>
+        </row>
+        <row r="15">
+          <cell r="G15">
+            <v>1</v>
+          </cell>
+        </row>
+        <row r="17">
+          <cell r="G17">
+            <v>6</v>
+          </cell>
+        </row>
+        <row r="18">
+          <cell r="G18">
+            <v>2</v>
+          </cell>
+        </row>
+        <row r="20">
+          <cell r="G20">
+            <v>2</v>
+          </cell>
+        </row>
+        <row r="21">
+          <cell r="G21">
+            <v>2</v>
+          </cell>
+        </row>
+        <row r="22">
+          <cell r="G22">
+            <v>6</v>
+          </cell>
+        </row>
+        <row r="23">
+          <cell r="G23">
+            <v>1.5</v>
+          </cell>
+        </row>
+        <row r="24">
+          <cell r="G24">
+            <v>2</v>
+          </cell>
+        </row>
+        <row r="26">
+          <cell r="G26">
+            <v>3</v>
+          </cell>
+        </row>
+        <row r="28">
+          <cell r="G28">
+            <v>2</v>
+          </cell>
+        </row>
+        <row r="29">
+          <cell r="G29">
+            <v>3</v>
+          </cell>
+        </row>
+        <row r="30">
+          <cell r="G30">
+            <v>1</v>
+          </cell>
+        </row>
+        <row r="31">
+          <cell r="G31">
+            <v>2</v>
+          </cell>
+        </row>
+        <row r="32">
+          <cell r="G32">
+            <v>3</v>
+          </cell>
+        </row>
+        <row r="33">
+          <cell r="G33">
+            <v>3</v>
+          </cell>
+        </row>
+        <row r="34">
+          <cell r="G34">
+            <v>5</v>
+          </cell>
+        </row>
+        <row r="35">
+          <cell r="G35">
+            <v>4.5</v>
+          </cell>
+        </row>
+        <row r="38">
+          <cell r="G38">
+            <v>5</v>
+          </cell>
+        </row>
+        <row r="39">
+          <cell r="G39">
+            <v>1.25</v>
+          </cell>
+        </row>
+        <row r="41">
+          <cell r="G41">
+            <v>3</v>
+          </cell>
+        </row>
+        <row r="42">
+          <cell r="G42">
+            <v>2</v>
+          </cell>
+        </row>
+        <row r="43">
+          <cell r="G43">
+            <v>2</v>
+          </cell>
+        </row>
+        <row r="44">
+          <cell r="G44">
+            <v>2</v>
+          </cell>
+        </row>
+        <row r="45">
+          <cell r="G45">
+            <v>2</v>
+          </cell>
+        </row>
+        <row r="46">
+          <cell r="G46">
+            <v>4.5</v>
+          </cell>
+        </row>
+        <row r="47">
+          <cell r="G47">
+            <v>2</v>
+          </cell>
+        </row>
+        <row r="48">
+          <cell r="G48">
+            <v>2.5</v>
+          </cell>
+        </row>
+      </sheetData>
+      <sheetData sheetId="2">
+        <row r="8">
+          <cell r="G8">
+            <v>3</v>
+          </cell>
+        </row>
+        <row r="10">
+          <cell r="G10">
+            <v>6</v>
+          </cell>
+        </row>
+        <row r="11">
+          <cell r="G11">
+            <v>2</v>
+          </cell>
+        </row>
+        <row r="14">
+          <cell r="G14">
+            <v>6</v>
+          </cell>
+        </row>
+        <row r="15">
+          <cell r="G15">
+            <v>2</v>
+          </cell>
+        </row>
+        <row r="17">
+          <cell r="G17">
+            <v>2</v>
+          </cell>
+        </row>
+        <row r="18">
+          <cell r="G18">
+            <v>6</v>
+          </cell>
+        </row>
+        <row r="19">
+          <cell r="G19">
+            <v>7.5</v>
+          </cell>
+        </row>
+        <row r="22">
+          <cell r="G22">
+            <v>3</v>
+          </cell>
+        </row>
+        <row r="23">
+          <cell r="G23">
+            <v>2.5</v>
+          </cell>
+        </row>
+        <row r="24">
+          <cell r="G24">
+            <v>3</v>
+          </cell>
+        </row>
+        <row r="25">
+          <cell r="G25">
+            <v>6</v>
+          </cell>
+        </row>
+        <row r="26">
+          <cell r="G26">
+            <v>6</v>
+          </cell>
+        </row>
+        <row r="27">
+          <cell r="G27">
+            <v>6</v>
+          </cell>
+        </row>
+        <row r="28">
+          <cell r="G28">
+            <v>3</v>
+          </cell>
+        </row>
+        <row r="29">
+          <cell r="G29">
+            <v>6</v>
+          </cell>
+        </row>
+        <row r="30">
+          <cell r="G30">
+            <v>7</v>
+          </cell>
+        </row>
+        <row r="31">
+          <cell r="G31">
+            <v>6</v>
+          </cell>
+        </row>
+        <row r="34">
+          <cell r="G34">
+            <v>6</v>
+          </cell>
+        </row>
+        <row r="35">
+          <cell r="G35">
+            <v>6</v>
+          </cell>
+        </row>
+        <row r="36">
+          <cell r="G36">
+            <v>1.25</v>
+          </cell>
+        </row>
+        <row r="37">
+          <cell r="G37">
+            <v>2</v>
+          </cell>
+        </row>
+      </sheetData>
+      <sheetData sheetId="3">
+        <row r="8">
+          <cell r="G8">
+            <v>3</v>
+          </cell>
+        </row>
+        <row r="10">
+          <cell r="G10">
+            <v>6</v>
+          </cell>
+        </row>
+        <row r="11">
+          <cell r="G11">
+            <v>1</v>
+          </cell>
+        </row>
+        <row r="13">
+          <cell r="G13">
+            <v>6</v>
+          </cell>
+        </row>
+        <row r="14">
+          <cell r="G14">
+            <v>2</v>
+          </cell>
+        </row>
+        <row r="15">
+          <cell r="G15">
+            <v>1.75</v>
+          </cell>
+        </row>
+        <row r="17">
+          <cell r="G17">
+            <v>2</v>
+          </cell>
+        </row>
+        <row r="18">
+          <cell r="G18">
+            <v>6</v>
+          </cell>
+        </row>
+        <row r="19">
+          <cell r="G19">
+            <v>4</v>
+          </cell>
+        </row>
+        <row r="22">
+          <cell r="G22">
+            <v>3</v>
+          </cell>
+        </row>
+        <row r="23">
+          <cell r="G23">
+            <v>2</v>
+          </cell>
+        </row>
+        <row r="24">
+          <cell r="G24">
+            <v>2</v>
+          </cell>
+        </row>
+        <row r="25">
+          <cell r="G25">
+            <v>3</v>
+          </cell>
+        </row>
+        <row r="26">
+          <cell r="G26">
+            <v>3.5</v>
+          </cell>
+        </row>
+        <row r="28">
+          <cell r="G28">
+            <v>4.5</v>
+          </cell>
+        </row>
+        <row r="29">
+          <cell r="G29">
+            <v>3</v>
+          </cell>
+        </row>
+        <row r="30">
+          <cell r="G30">
+            <v>4</v>
+          </cell>
+        </row>
+        <row r="31">
+          <cell r="G31">
+            <v>4</v>
+          </cell>
+        </row>
+        <row r="35">
+          <cell r="G35">
+            <v>1.25</v>
+          </cell>
+        </row>
+        <row r="36">
+          <cell r="G36">
+            <v>2</v>
+          </cell>
+        </row>
+        <row r="38">
+          <cell r="G38">
+            <v>3.25</v>
+          </cell>
+        </row>
+        <row r="39">
+          <cell r="G39">
+            <v>1.75</v>
+          </cell>
+        </row>
+        <row r="41">
+          <cell r="G41">
+            <v>4.5</v>
+          </cell>
+        </row>
+      </sheetData>
+      <sheetData sheetId="4">
+        <row r="8">
+          <cell r="G8">
+            <v>3</v>
+          </cell>
+        </row>
+        <row r="10">
+          <cell r="G10">
+            <v>6</v>
+          </cell>
+        </row>
+        <row r="11">
+          <cell r="G11">
+            <v>2</v>
+          </cell>
+        </row>
+        <row r="13">
+          <cell r="G13">
+            <v>1.5</v>
+          </cell>
+        </row>
+        <row r="15">
+          <cell r="G15">
+            <v>6</v>
+          </cell>
+        </row>
+        <row r="16">
+          <cell r="G16">
+            <v>2</v>
+          </cell>
+        </row>
+        <row r="17">
+          <cell r="G17">
+            <v>1.5</v>
+          </cell>
+        </row>
+        <row r="19">
+          <cell r="G19">
+            <v>2</v>
+          </cell>
+        </row>
+        <row r="20">
+          <cell r="G20">
+            <v>6</v>
+          </cell>
+        </row>
+        <row r="21">
+          <cell r="G21">
+            <v>7.5</v>
+          </cell>
+        </row>
+        <row r="23">
+          <cell r="G23">
+            <v>1.5</v>
+          </cell>
+        </row>
+        <row r="24">
+          <cell r="G24">
+            <v>3</v>
+          </cell>
+        </row>
+        <row r="25">
+          <cell r="G25">
+            <v>2.5</v>
+          </cell>
+        </row>
+        <row r="26">
+          <cell r="G26">
+            <v>3</v>
+          </cell>
+        </row>
+        <row r="27">
+          <cell r="G27">
+            <v>6</v>
+          </cell>
+        </row>
+        <row r="28">
+          <cell r="G28">
+            <v>6</v>
+          </cell>
+        </row>
+        <row r="29">
+          <cell r="G29">
+            <v>6</v>
+          </cell>
+        </row>
+        <row r="31">
+          <cell r="G31">
+            <v>6</v>
+          </cell>
+        </row>
+        <row r="32">
+          <cell r="G32">
+            <v>7</v>
+          </cell>
+        </row>
+        <row r="33">
+          <cell r="G33">
+            <v>6</v>
+          </cell>
+        </row>
+        <row r="36">
+          <cell r="G36">
+            <v>6</v>
+          </cell>
+        </row>
+        <row r="37">
+          <cell r="G37">
+            <v>6</v>
+          </cell>
+        </row>
+        <row r="38">
+          <cell r="G38">
+            <v>1.25</v>
+          </cell>
+        </row>
+        <row r="39">
+          <cell r="G39">
+            <v>2</v>
+          </cell>
+        </row>
+      </sheetData>
+    </sheetDataSet>
+  </externalBook>
+</externalLink>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -460,8 +1008,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A58A5F59-6792-4D16-B0A7-C65959325E3B}">
   <dimension ref="A1:D16"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G17" sqref="G17"/>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:B15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -621,4 +1169,355 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BCBFD6D3-C5ED-4569-95FC-28394E5122A1}">
+  <dimension ref="A1:G16"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E17" sqref="E17"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="49.140625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="12" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>12</v>
+      </c>
+      <c r="C1" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="C2" t="s">
+        <v>14</v>
+      </c>
+      <c r="D2" t="s">
+        <v>16</v>
+      </c>
+      <c r="E2" t="s">
+        <v>20</v>
+      </c>
+      <c r="F2" t="s">
+        <v>19</v>
+      </c>
+      <c r="G2" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>1</v>
+      </c>
+      <c r="B3">
+        <v>50</v>
+      </c>
+      <c r="C3">
+        <f>SUM(D3:G3)</f>
+        <v>51.5</v>
+      </c>
+      <c r="D3">
+        <f>[1]Aistleithner!$G$8+[1]Aistleithner!$G$10+[1]Aistleithner!$G$31+[1]Aistleithner!$G$32+[1]Aistleithner!$G$33+[1]Aistleithner!$G$39+[1]Aistleithner!$G$43</f>
+        <v>16.25</v>
+      </c>
+      <c r="E3">
+        <f>[1]Dusanic!$G$8+[1]Dusanic!$G$24+[1]Dusanic!$G$28+[1]Dusanic!$G$36+[1]Dusanic!$G$37</f>
+        <v>12.25</v>
+      </c>
+      <c r="F3">
+        <f>SUM([1]Teuchtmann!$G$8+[1]Teuchtmann!$G$25+[1]Teuchtmann!$G$29+[1]Teuchtmann!$G$35+[1]Teuchtmann!$G$36)</f>
+        <v>12.25</v>
+      </c>
+      <c r="G3">
+        <f>SUM([1]Tomic!$G$8+[1]Tomic!$G$23+[1]Tomic!$G$26+[1]Tomic!$G$38+[1]Tomic!$G$39)</f>
+        <v>10.75</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>2</v>
+      </c>
+      <c r="B4">
+        <v>50</v>
+      </c>
+      <c r="C4">
+        <f t="shared" ref="C4:C14" si="0">SUM(D4:G4)</f>
+        <v>151.75</v>
+      </c>
+      <c r="D4">
+        <f>SUM([1]Aistleithner!$G$11+[1]Aistleithner!$G$12+[1]Aistleithner!$G$14+[1]Aistleithner!$G$15+[1]Aistleithner!$G$17+[1]Aistleithner!$G$18+[1]Aistleithner!$G$21+[1]Aistleithner!$G$20+[1]Aistleithner!$G$22+[1]Aistleithner!$G$23+[1]Aistleithner!$G$24++[1]Aistleithner!$G$26+[1]Aistleithner!$G$28+[1]Aistleithner!$G$29+[1]Aistleithner!$G$30+[1]Aistleithner!$G$31)</f>
+        <v>43</v>
+      </c>
+      <c r="E4">
+        <f>SUM([1]Dusanic!$G$10+[1]Dusanic!$G$11+[1]Dusanic!$G$14+[1]Dusanic!$G$15+[1]Dusanic!$G$17+[1]Dusanic!$G$18+[1]Dusanic!$G$19+[1]Dusanic!$G$22+[1]Dusanic!$G$23)</f>
+        <v>37</v>
+      </c>
+      <c r="F4">
+        <f>SUM([1]Teuchtmann!$G$10+[1]Teuchtmann!$G$11+[1]Teuchtmann!$G$13+[1]Teuchtmann!$G$15+[1]Teuchtmann!$G$17+[1]Teuchtmann!$G$18+[1]Teuchtmann!$G$19+[1]Teuchtmann!$G$22+[1]Teuchtmann!$G$23)</f>
+        <v>31.75</v>
+      </c>
+      <c r="G4">
+        <f>SUM([1]Tomic!$G$10+[1]Tomic!$G$11+[1]Tomic!$G$13+[1]Tomic!$G$15+[1]Tomic!$G$16+[1]Tomic!$G$17+[1]Tomic!$G$19+[1]Tomic!$G$20+[1]Tomic!$G$21+[1]Tomic!$G$24+[1]Tomic!$G$25)</f>
+        <v>40</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A5" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="C5">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>3</v>
+      </c>
+      <c r="B6">
+        <v>50</v>
+      </c>
+      <c r="C6">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="D6">
+        <v>0</v>
+      </c>
+      <c r="E6">
+        <v>0</v>
+      </c>
+      <c r="F6">
+        <v>0</v>
+      </c>
+      <c r="G6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>4</v>
+      </c>
+      <c r="B7">
+        <v>140</v>
+      </c>
+      <c r="C7">
+        <f t="shared" si="0"/>
+        <v>98</v>
+      </c>
+      <c r="D7">
+        <v>0</v>
+      </c>
+      <c r="E7">
+        <f>SUM([1]Dusanic!$G$25+[1]Dusanic!$G$26+[1]Dusanic!$G$27+[1]Dusanic!$G$29+[1]Dusanic!$G$30+[1]Dusanic!$G$31+[1]Dusanic!$G$34+[1]Dusanic!$G$35)</f>
+        <v>49</v>
+      </c>
+      <c r="F7">
+        <v>0</v>
+      </c>
+      <c r="G7">
+        <f>SUM([1]Tomic!$G$27+[1]Tomic!$G$28+[1]Tomic!$G$29+[1]Tomic!$G$31+[1]Tomic!$G$32+[1]Tomic!$G$33+[1]Tomic!$G$36+[1]Tomic!$G$37)</f>
+        <v>49</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>5</v>
+      </c>
+      <c r="B8">
+        <v>100</v>
+      </c>
+      <c r="C8">
+        <f t="shared" si="0"/>
+        <v>28</v>
+      </c>
+      <c r="D8">
+        <f>SUM([1]Aistleithner!$G$34+[1]Aistleithner!$G$35+[1]Aistleithner!$G$38+[1]Aistleithner!$G$41+[1]Aistleithner!$G$42+[1]Aistleithner!$G$44+[1]Aistleithner!$G$46+[1]Aistleithner!$G$47)</f>
+        <v>28</v>
+      </c>
+      <c r="E8">
+        <v>0</v>
+      </c>
+      <c r="F8">
+        <v>0</v>
+      </c>
+      <c r="G8">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>6</v>
+      </c>
+      <c r="B9">
+        <v>30</v>
+      </c>
+      <c r="C9">
+        <f t="shared" si="0"/>
+        <v>25</v>
+      </c>
+      <c r="D9">
+        <v>0</v>
+      </c>
+      <c r="E9">
+        <v>0</v>
+      </c>
+      <c r="F9">
+        <f>SUM([1]Teuchtmann!$G$14+[1]Teuchtmann!$G$24+[1]Teuchtmann!$G$26+[1]Teuchtmann!$G$30+[1]Teuchtmann!$G$31+[1]Teuchtmann!$G$38+[1]Teuchtmann!$G$39+[1]Teuchtmann!$G$41)</f>
+        <v>25</v>
+      </c>
+      <c r="G9">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>7</v>
+      </c>
+      <c r="B10">
+        <v>50</v>
+      </c>
+      <c r="C10">
+        <f t="shared" si="0"/>
+        <v>2</v>
+      </c>
+      <c r="D10">
+        <f>[1]Aistleithner!$G$45</f>
+        <v>2</v>
+      </c>
+      <c r="E10">
+        <v>0</v>
+      </c>
+      <c r="F10">
+        <v>0</v>
+      </c>
+      <c r="G10">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>8</v>
+      </c>
+      <c r="B11">
+        <v>40</v>
+      </c>
+      <c r="C11">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="D11">
+        <v>0</v>
+      </c>
+      <c r="E11">
+        <v>0</v>
+      </c>
+      <c r="F11">
+        <v>0</v>
+      </c>
+      <c r="G11">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>11</v>
+      </c>
+      <c r="B12">
+        <v>40</v>
+      </c>
+      <c r="C12">
+        <f t="shared" si="0"/>
+        <v>2</v>
+      </c>
+      <c r="D12">
+        <f>[1]Aistleithner!$G$44</f>
+        <v>2</v>
+      </c>
+      <c r="E12">
+        <v>0</v>
+      </c>
+      <c r="F12">
+        <v>0</v>
+      </c>
+      <c r="G12">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>9</v>
+      </c>
+      <c r="B13">
+        <v>30</v>
+      </c>
+      <c r="C13">
+        <f t="shared" si="0"/>
+        <v>9.5</v>
+      </c>
+      <c r="D13">
+        <f>[1]Aistleithner!$G$45</f>
+        <v>2</v>
+      </c>
+      <c r="E13">
+        <v>0</v>
+      </c>
+      <c r="F13">
+        <f>[1]Teuchtmann!$G$28+[1]Teuchtmann!$G$29</f>
+        <v>7.5</v>
+      </c>
+      <c r="G13">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>10</v>
+      </c>
+      <c r="B14">
+        <v>30</v>
+      </c>
+      <c r="C14">
+        <f t="shared" si="0"/>
+        <v>2.5</v>
+      </c>
+      <c r="D14">
+        <f>SUM([1]Aistleithner!$G$48)</f>
+        <v>2.5</v>
+      </c>
+      <c r="E14">
+        <v>0</v>
+      </c>
+      <c r="F14">
+        <v>0</v>
+      </c>
+      <c r="G14">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A15" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="B15" s="2">
+        <f>SUM(B3:B14)</f>
+        <v>610</v>
+      </c>
+      <c r="C15" s="2">
+        <f>SUM(C3:C14)</f>
+        <v>370.25</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" ht="15.75" thickTop="1" x14ac:dyDescent="0.25"/>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>